<commit_message>
upates for conveyor belt adaptability
</commit_message>
<xml_diff>
--- a/Workspace Co-ordinates RS D415 Conveyor Belt.xlsx
+++ b/Workspace Co-ordinates RS D415 Conveyor Belt.xlsx
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="103" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
conveyor belt pickup updates
</commit_message>
<xml_diff>
--- a/Workspace Co-ordinates RS D415 Conveyor Belt.xlsx
+++ b/Workspace Co-ordinates RS D415 Conveyor Belt.xlsx
@@ -742,7 +742,7 @@
   <dimension ref="A2:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,18 +771,16 @@
         <v>4</v>
       </c>
       <c r="I3" s="1">
-        <f>0.349+0.32</f>
-        <v>0.66900000000000004</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="J3" s="1">
-        <f>0.359+0.32</f>
-        <v>0.67900000000000005</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="K3" s="1">
-        <v>0.187</v>
+        <v>0.184</v>
       </c>
       <c r="L3" s="1">
-        <v>0.191</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -790,16 +788,16 @@
         <v>5</v>
       </c>
       <c r="I4" s="1">
-        <v>0.16600000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="J4" s="1">
-        <v>-2.8000000000000001E-2</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="K4" s="1">
-        <v>-2.8000000000000001E-2</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="L4" s="1">
-        <v>0.16600000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -807,16 +805,16 @@
         <v>6</v>
       </c>
       <c r="I5" s="1">
-        <v>2E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="J5" s="1">
-        <v>2E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="K5" s="1">
-        <v>2E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="L5" s="1">
-        <v>2E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -824,16 +822,16 @@
         <v>7</v>
       </c>
       <c r="I6" s="1">
-        <v>-2.6019999999999999</v>
+        <v>3.12</v>
       </c>
       <c r="J6" s="1">
-        <v>3.1339999999999999</v>
+        <v>3.12</v>
       </c>
       <c r="K6" s="1">
-        <v>2.8330000000000002</v>
+        <v>3.12</v>
       </c>
       <c r="L6" s="1">
-        <v>-0.215</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -841,16 +839,16 @@
         <v>8</v>
       </c>
       <c r="I7" s="1">
-        <v>0.96</v>
+        <v>1.444</v>
       </c>
       <c r="J7" s="1">
-        <v>1.115</v>
+        <v>1.44</v>
       </c>
       <c r="K7" s="1">
-        <v>1.4710000000000001</v>
+        <v>1.44</v>
       </c>
       <c r="L7" s="1">
-        <v>1.0780000000000001</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -858,16 +856,16 @@
         <v>9</v>
       </c>
       <c r="I8" s="1">
-        <v>0.5</v>
+        <v>3.032</v>
       </c>
       <c r="J8" s="1">
-        <v>-7.0999999999999994E-2</v>
+        <v>3.032</v>
       </c>
       <c r="K8" s="1">
-        <v>2.2690000000000001</v>
+        <v>3.032</v>
       </c>
       <c r="L8" s="1">
-        <v>2.2690000000000001</v>
+        <v>3.032</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated conveyor belt code
</commit_message>
<xml_diff>
--- a/Workspace Co-ordinates RS D415 Conveyor Belt.xlsx
+++ b/Workspace Co-ordinates RS D415 Conveyor Belt.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Point 1</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Yaw</t>
-  </si>
-  <si>
-    <t>Points 1 and 2 have x value calculated mathematically</t>
   </si>
 </sst>
 </file>
@@ -105,9 +102,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,16 +376,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -399,7 +394,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="411480" y="1470660"/>
+          <a:off x="4114800" y="1478280"/>
           <a:ext cx="15240" cy="2011680"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -428,16 +423,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -445,9 +440,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="426720" y="3482340"/>
-          <a:ext cx="1996440" cy="7620"/>
+        <a:xfrm flipH="1">
+          <a:off x="2423160" y="3482340"/>
+          <a:ext cx="1691640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -739,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R20"/>
+  <dimension ref="E2:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +746,7 @@
     <col min="10" max="10" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -766,117 +761,115 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="1">
-        <v>0.72499999999999998</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="J3" s="1">
-        <v>0.72499999999999998</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="K3" s="1">
-        <v>0.184</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="L3" s="1">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.17699999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="1">
-        <v>0.18099999999999999</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="J4" s="1">
-        <v>-1.9E-2</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="K4" s="1">
-        <v>-1.9E-2</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="L4" s="1">
-        <v>0.18099999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="1">
-        <v>-4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>-4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>-4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>-4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="1">
-        <v>3.12</v>
+        <v>3.0939999999999999</v>
       </c>
       <c r="J6" s="1">
-        <v>3.12</v>
+        <v>3.0939999999999999</v>
       </c>
       <c r="K6" s="1">
-        <v>3.12</v>
+        <v>3.0939999999999999</v>
       </c>
       <c r="L6" s="1">
-        <v>3.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>3.0939999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="1">
-        <v>1.444</v>
+        <v>1.5189999999999999</v>
       </c>
       <c r="J7" s="1">
-        <v>1.44</v>
+        <v>1.5189999999999999</v>
       </c>
       <c r="K7" s="1">
-        <v>1.44</v>
+        <v>1.5189999999999999</v>
       </c>
       <c r="L7" s="1">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1.5189999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="1">
-        <v>3.032</v>
+        <v>3.06</v>
       </c>
       <c r="J8" s="1">
-        <v>3.032</v>
+        <v>3.06</v>
       </c>
       <c r="K8" s="1">
-        <v>3.032</v>
+        <v>3.06</v>
       </c>
       <c r="L8" s="1">
-        <v>3.032</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="10" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J15" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="15" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -886,15 +879,12 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J15:R15"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>